<commit_message>
Return TC 1 to 10
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Return/adhoc_return_test_data.xlsx
+++ b/TestData/Web_POS/Return/adhoc_return_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="45">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -67,16 +67,22 @@
     <t xml:space="preserve">group</t>
   </si>
   <si>
-    <t xml:space="preserve">TC_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">307260624WoJ</t>
+    <t xml:space="preserve">Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">salesperson_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">307260624P3E</t>
   </si>
   <si>
     <t xml:space="preserve">zwshashank.agrawal@teampureplay.com</t>
   </si>
   <si>
-    <t xml:space="preserve">usertwo_p1</t>
+    <t xml:space="preserve">userone_p1 </t>
   </si>
   <si>
     <t xml:space="preserve">Index9QA</t>
@@ -97,16 +103,76 @@
     <t xml:space="preserve">Dummy</t>
   </si>
   <si>
-    <t xml:space="preserve">TC_02</t>
+    <t xml:space="preserve">Return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">307260624ut0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">userone_p2</t>
   </si>
   <si>
     <t xml:space="preserve">Alexa67 : 1</t>
   </si>
   <si>
-    <t xml:space="preserve">TC_03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_04</t>
+    <t xml:space="preserve">R_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TSAL00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saloni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_9</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8906118410781 : 1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">8906118410781 : 1</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">R_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_12</t>
   </si>
 </sst>
 </file>
@@ -117,7 +183,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -151,6 +217,24 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,7 +279,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,8 +292,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -229,15 +325,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -286,22 +391,28 @@
       <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
+      <c r="E2" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>123456</v>
@@ -313,42 +424,45 @@
         <v>500</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>45384</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>18</v>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>123456</v>
@@ -360,42 +474,45 @@
         <v>500</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="3" t="n">
-        <v>45384</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="L3" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>123456</v>
@@ -407,42 +524,45 @@
         <v>300</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="3" t="n">
-        <v>45384</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>123456</v>
@@ -454,26 +574,439 @@
         <v>400</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="3" t="n">
-        <v>45384</v>
-      </c>
-      <c r="M5" s="3" t="s">
+      <c r="F6" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="K6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H11" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q13" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Return Testcases 1 to 24
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Return/adhoc_return_test_data.xlsx
+++ b/TestData/Web_POS/Return/adhoc_return_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="56">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">salesperson_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assortment</t>
   </si>
   <si>
     <t xml:space="preserve">R_1</t>
@@ -173,6 +176,36 @@
   </si>
   <si>
     <t xml:space="preserve">R_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8906118410781 : 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">307260624buU </t>
+  </si>
+  <si>
+    <t xml:space="preserve">userone_p9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_19</t>
   </si>
 </sst>
 </file>
@@ -325,10 +358,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -342,7 +375,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,22 +432,25 @@
       <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>123456</v>
@@ -424,45 +462,45 @@
         <v>500</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>123456</v>
@@ -474,45 +512,45 @@
         <v>500</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L3" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>123456</v>
@@ -524,45 +562,45 @@
         <v>300</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L4" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>123456</v>
@@ -574,45 +612,45 @@
         <v>400</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L5" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>123456</v>
@@ -624,46 +662,46 @@
         <v>400</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L6" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>123456</v>
@@ -675,46 +713,46 @@
         <v>400</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L7" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>123456</v>
@@ -726,46 +764,49 @@
         <v>400</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L8" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q8" s="6"/>
+      <c r="R8" s="6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>123456</v>
@@ -777,48 +818,48 @@
         <v>400</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L9" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="n">
         <v>123456</v>
@@ -830,97 +871,97 @@
         <v>400</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L10" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H11" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G11" s="6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H11" s="6" t="n">
-        <v>400</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="K11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L11" s="4" t="n">
         <v>45384</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="n">
         <v>123456</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" s="1" t="n">
         <v>123456</v>
@@ -932,81 +973,457 @@
         <v>400</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H14" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="4" t="n">
-        <v>45384</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P12" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="1" t="n">
-        <v>123456</v>
-      </c>
-      <c r="G13" s="6" t="n">
-        <v>1000</v>
-      </c>
-      <c r="H13" s="6" t="n">
-        <v>400</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="2" t="s">
+      <c r="K14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H15" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="4" t="n">
-        <v>45384</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q13" s="6"/>
+      <c r="K15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H16" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H17" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L17" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H18" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q18" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H19" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q19" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G20" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H20" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Debugged TC 22 to 25
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Return/adhoc_return_test_data.xlsx
+++ b/TestData/Web_POS/Return/adhoc_return_test_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="72">
   <si>
     <t xml:space="preserve">TC_Id</t>
   </si>
@@ -187,15 +187,53 @@
     <t xml:space="preserve">R_14</t>
   </si>
   <si>
+    <t xml:space="preserve">307260624Wa9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">userone_p10</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8906118410781 : 1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">8906118412556</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve"> : 1, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">8906118412662:1</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">R_15</t>
   </si>
   <si>
-    <t xml:space="preserve">307260624buU </t>
-  </si>
-  <si>
-    <t xml:space="preserve">userone_p9 </t>
-  </si>
-  <si>
     <t xml:space="preserve">R_16</t>
   </si>
   <si>
@@ -206,6 +244,51 @@
   </si>
   <si>
     <t xml:space="preserve">R_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_34</t>
   </si>
 </sst>
 </file>
@@ -216,7 +299,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -268,6 +351,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,10 +447,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -374,7 +463,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.44"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="36.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="11" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
@@ -845,7 +934,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>41</v>
       </c>
@@ -896,7 +985,7 @@
       </c>
       <c r="Q10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
@@ -1001,7 +1090,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
@@ -1104,12 +1193,12 @@
       </c>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>19</v>
+      <c r="B15" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
@@ -1118,7 +1207,7 @@
         <v>123456</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>123456</v>
@@ -1133,7 +1222,7 @@
         <v>22</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>24</v>
@@ -1162,10 +1251,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>20</v>
@@ -1174,7 +1263,7 @@
         <v>123456</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>123456</v>
@@ -1215,7 +1304,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>19</v>
@@ -1268,7 +1357,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>19</v>
@@ -1321,7 +1410,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>
@@ -1374,7 +1463,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>19</v>
@@ -1423,6 +1512,756 @@
       </c>
       <c r="Q20" s="6" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H21" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G22" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H22" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G23" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H23" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G24" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H24" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P24" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G25" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G26" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H26" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G27" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H27" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L27" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P27" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G28" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H28" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L28" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G29" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H29" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G30" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H30" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L30" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P30" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H31" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G32" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H32" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L32" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G33" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H33" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L33" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G34" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H34" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L34" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>123456</v>
+      </c>
+      <c r="G35" s="6" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H35" s="6" t="n">
+        <v>400</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L35" s="4" t="n">
+        <v>45384</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P35" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test data for TC 15
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Return/adhoc_return_test_data.xlsx
+++ b/TestData/Web_POS/Return/adhoc_return_test_data.xlsx
@@ -148,25 +148,7 @@
     <t xml:space="preserve">R_9</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8906118410781 : 1, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">8906118410781 : 1</t>
-    </r>
+    <t xml:space="preserve">8906118410781 : 1, 8906118410781 : 1</t>
   </si>
   <si>
     <t xml:space="preserve">R_10</t>
@@ -209,6 +191,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8906118412556</t>
     </r>
@@ -217,6 +200,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> : 1, </t>
     </r>
@@ -226,6 +210,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">8906118412662:1</t>
     </r>
@@ -299,11 +284,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]M/D/YYYY"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -336,27 +322,23 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -414,7 +396,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,7 +404,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -450,7 +432,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -459,9 +441,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="36.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="11" style="0" width="11.52"/>
@@ -1254,7 +1236,7 @@
         <v>52</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>20</v>
@@ -1263,7 +1245,7 @@
         <v>123456</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>123456</v>

</xml_diff>